<commit_message>
Major update: code cleaning + adding documentation (github pages)
</commit_message>
<xml_diff>
--- a/data/MBP.xlsx
+++ b/data/MBP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\LT-AoP-22\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\R\LT-AoP-22-Book\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0676ED-6378-4CA7-9187-632D95EFF0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBC07D8-76F4-4D8C-B412-94FB13FD27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mbp" sheetId="2" r:id="rId1"/>
@@ -1190,20 +1190,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="L255" sqref="L255"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.84375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.61328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.84375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>261</v>
       </c>
@@ -1227,7 +1229,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>26855.868709999984</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>36236.316373000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>33246.669505999969</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>262</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>30536.491911000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>262</v>
       </c>
@@ -1342,7 +1344,7 @@
         <v>47446.570896199941</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>262</v>
       </c>
@@ -1365,7 +1367,7 @@
         <v>42413.079165299954</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>262</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>48415.338636</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>262</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>41249.949720299941</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>262</v>
       </c>
@@ -1434,7 +1436,7 @@
         <v>34805.734646999983</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>262</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>41588.384261000057</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>262</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>52494.512606000062</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>44302.837843000052</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>262</v>
       </c>
@@ -1526,7 +1528,7 @@
         <v>41415.388175999979</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>262</v>
       </c>
@@ -1549,7 +1551,7 @@
         <v>41761.405426999983</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>262</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>22389.059843999967</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>262</v>
       </c>
@@ -1595,7 +1597,7 @@
         <v>15884.823321999995</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>262</v>
       </c>
@@ -1618,7 +1620,7 @@
         <v>25974.084919999998</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>31172.677027000002</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>262</v>
       </c>
@@ -1664,7 +1666,7 @@
         <v>35974.204694999964</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>262</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>39525.247889999984</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>262</v>
       </c>
@@ -1710,7 +1712,7 @@
         <v>30177.466952600022</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>262</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>27951.624693000012</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>262</v>
       </c>
@@ -1756,7 +1758,7 @@
         <v>30029.891168499962</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>262</v>
       </c>
@@ -1779,7 +1781,7 @@
         <v>29419.594360000006</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>262</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>42561.253270999943</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>262</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>28361.909360000016</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>262</v>
       </c>
@@ -1848,7 +1850,7 @@
         <v>26054.600760999991</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>262</v>
       </c>
@@ -1856,7 +1858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>262</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>51499.48455700004</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>262</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>59647.87574999989</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>262</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>69671.606896999961</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>262</v>
       </c>
@@ -1938,7 +1940,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>262</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>49487.197367000124</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>262</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>42932.64872969994</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>262</v>
       </c>
@@ -2007,7 +2009,7 @@
         <v>33897.969448000011</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>262</v>
       </c>
@@ -2015,7 +2017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>262</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>28861.566094500013</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>262</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>17483.42532100001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>262</v>
       </c>
@@ -2084,7 +2086,7 @@
         <v>47783.484962999959</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>262</v>
       </c>
@@ -2092,7 +2094,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>262</v>
       </c>
@@ -2115,7 +2117,7 @@
         <v>22740.860398999987</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>262</v>
       </c>
@@ -2138,7 +2140,7 @@
         <v>26209.423306000019</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>262</v>
       </c>
@@ -2161,7 +2163,7 @@
         <v>29998.117587999972</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>262</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>262</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>13098.701186999993</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>262</v>
       </c>
@@ -2215,7 +2217,7 @@
         <v>15018.175139999996</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>262</v>
       </c>
@@ -2238,7 +2240,7 @@
         <v>55214.510262000062</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>262</v>
       </c>
@@ -2246,7 +2248,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>262</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>38713.007128999969</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>262</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>54228.661629000038</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>262</v>
       </c>
@@ -2315,7 +2317,7 @@
         <v>26354.343889399988</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>262</v>
       </c>
@@ -2338,7 +2340,7 @@
         <v>66967.78593579997</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>262</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>46319.388708999992</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>262</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>42705.423975999969</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>262</v>
       </c>
@@ -2407,7 +2409,7 @@
         <v>15104.604628000006</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>262</v>
       </c>
@@ -2430,7 +2432,7 @@
         <v>51922.182475000001</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>262</v>
       </c>
@@ -2453,7 +2455,7 @@
         <v>47079.948170400028</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -2476,7 +2478,7 @@
         <v>49880.626503</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -2499,7 +2501,7 @@
         <v>45599.339338899939</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>262</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>67450.635794000089</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -2545,7 +2547,7 @@
         <v>73471.918864000123</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -2568,7 +2570,7 @@
         <v>65148.948371999992</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>262</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>58336.977065999985</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>262</v>
       </c>
@@ -2614,7 +2616,7 @@
         <v>51677.557368000016</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>262</v>
       </c>
@@ -2637,7 +2639,7 @@
         <v>46942.248373000031</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>262</v>
       </c>
@@ -2660,7 +2662,7 @@
         <v>40611.322574999969</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>262</v>
       </c>
@@ -2683,7 +2685,7 @@
         <v>32375.80037600005</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>262</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>33323.550794999966</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>262</v>
       </c>
@@ -2729,7 +2731,7 @@
         <v>52555.875265999937</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>262</v>
       </c>
@@ -2752,7 +2754,7 @@
         <v>31460.067431000014</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>262</v>
       </c>
@@ -2775,7 +2777,7 @@
         <v>32982.604945000021</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>262</v>
       </c>
@@ -2798,7 +2800,7 @@
         <v>31410.139293300024</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>262</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>35341.681830999943</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>262</v>
       </c>
@@ -2844,7 +2846,7 @@
         <v>60977.751716999977</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>262</v>
       </c>
@@ -2867,7 +2869,7 @@
         <v>50139.561406999957</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>34148.020262999977</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>262</v>
       </c>
@@ -2913,7 +2915,7 @@
         <v>35095.486531000024</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>262</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>71738.142483600022</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>262</v>
       </c>
@@ -2959,7 +2961,7 @@
         <v>50128.351453999989</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>262</v>
       </c>
@@ -2982,7 +2984,7 @@
         <v>35269.404827299957</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>262</v>
       </c>
@@ -3005,7 +3007,7 @@
         <v>23802.311727999964</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>262</v>
       </c>
@@ -3028,7 +3030,7 @@
         <v>36313.781963999973</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>262</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>35306.395338299953</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>262</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>30687.089936999964</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>262</v>
       </c>
@@ -3097,7 +3099,7 @@
         <v>39869.904093000056</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>262</v>
       </c>
@@ -3120,7 +3122,7 @@
         <v>36198.320382300022</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>262</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>24581.76138099996</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>262</v>
       </c>
@@ -3166,7 +3168,7 @@
         <v>47855.965265499959</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>262</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>39880.724252000015</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>262</v>
       </c>
@@ -3212,7 +3214,7 @@
         <v>57521.165088000016</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>262</v>
       </c>
@@ -3235,7 +3237,7 @@
         <v>35745.570995999973</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>262</v>
       </c>
@@ -3243,7 +3245,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>262</v>
       </c>
@@ -3266,7 +3268,7 @@
         <v>72140.029592999999</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>262</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>51125.842587000079</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>262</v>
       </c>
@@ -3312,7 +3314,7 @@
         <v>66416.975373999943</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>262</v>
       </c>
@@ -3335,7 +3337,7 @@
         <v>46699.111703299939</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>262</v>
       </c>
@@ -3358,7 +3360,7 @@
         <v>17835.970864999996</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>262</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>34174.808282899969</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>262</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>50833.395862999998</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>262</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>31411.362429000004</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>262</v>
       </c>
@@ -3450,7 +3452,7 @@
         <v>31920.204148000052</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>262</v>
       </c>
@@ -3473,7 +3475,7 @@
         <v>18908.048459999995</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>262</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>41006.347018000008</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>262</v>
       </c>
@@ -3519,7 +3521,7 @@
         <v>30328.250261300003</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>262</v>
       </c>
@@ -3542,7 +3544,7 @@
         <v>26464.918454999977</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>262</v>
       </c>
@@ -3565,7 +3567,7 @@
         <v>37092.005063000019</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>262</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>27238.630400000016</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>262</v>
       </c>
@@ -3611,7 +3613,7 @@
         <v>58803.73888599997</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>262</v>
       </c>
@@ -3634,7 +3636,7 @@
         <v>33152.042082000036</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>262</v>
       </c>
@@ -3657,7 +3659,7 @@
         <v>32742.836483999996</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>262</v>
       </c>
@@ -3680,7 +3682,7 @@
         <v>38979.305495000037</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>262</v>
       </c>
@@ -3703,7 +3705,7 @@
         <v>34589.818702000048</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>262</v>
       </c>
@@ -3726,7 +3728,7 @@
         <v>20068.106400999975</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>262</v>
       </c>
@@ -3749,7 +3751,7 @@
         <v>23946.710903000014</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>262</v>
       </c>
@@ -3772,7 +3774,7 @@
         <v>32839.324934000018</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>262</v>
       </c>
@@ -3795,7 +3797,7 @@
         <v>39327.083586500026</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>262</v>
       </c>
@@ -3818,7 +3820,7 @@
         <v>39814.832854999971</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>262</v>
       </c>
@@ -3841,7 +3843,7 @@
         <v>48231.096277900077</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>262</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>20414.933852999988</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>262</v>
       </c>
@@ -3887,7 +3889,7 @@
         <v>46791.217666999881</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>262</v>
       </c>
@@ -3910,7 +3912,7 @@
         <v>18587.40689599999</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>262</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>36900.211931699967</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>262</v>
       </c>
@@ -3956,7 +3958,7 @@
         <v>28509.020528000015</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>262</v>
       </c>
@@ -3979,7 +3981,7 @@
         <v>28358.728157000023</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>262</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>49305.051588999988</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>262</v>
       </c>
@@ -4025,7 +4027,7 @@
         <v>47617.567492999937</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>262</v>
       </c>
@@ -4048,7 +4050,7 @@
         <v>23174.335484400002</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>262</v>
       </c>
@@ -4071,7 +4073,7 @@
         <v>51691.461505999956</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>262</v>
       </c>
@@ -4094,7 +4096,7 @@
         <v>74252.140289299976</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>262</v>
       </c>
@@ -4117,7 +4119,7 @@
         <v>58539.165246000084</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -4125,7 +4127,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>262</v>
       </c>
@@ -4148,7 +4150,7 @@
         <v>51090.962175000059</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>262</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>70184.967247999986</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>262</v>
       </c>
@@ -4194,7 +4196,7 @@
         <v>70325.928039499966</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>262</v>
       </c>
@@ -4202,7 +4204,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>262</v>
       </c>
@@ -4225,7 +4227,7 @@
         <v>66453.745005999997</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>262</v>
       </c>
@@ -4248,7 +4250,7 @@
         <v>66836.609006499872</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>262</v>
       </c>
@@ -4271,7 +4273,7 @@
         <v>60924.483507999939</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>262</v>
       </c>
@@ -4279,7 +4281,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>262</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>68367.176665999956</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>262</v>
       </c>
@@ -4325,7 +4327,7 @@
         <v>77840.528497000181</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>262</v>
       </c>
@@ -4348,7 +4350,7 @@
         <v>78828.904265299847</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>262</v>
       </c>
@@ -4356,7 +4358,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>262</v>
       </c>
@@ -4379,7 +4381,7 @@
         <v>21549.342100000009</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>262</v>
       </c>
@@ -4402,7 +4404,7 @@
         <v>16870.970648999988</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>262</v>
       </c>
@@ -4425,7 +4427,7 @@
         <v>23560.250986000032</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>262</v>
       </c>
@@ -4448,7 +4450,7 @@
         <v>16248.537338999995</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>262</v>
       </c>
@@ -4471,7 +4473,7 @@
         <v>23889.291300699992</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>262</v>
       </c>
@@ -4494,7 +4496,7 @@
         <v>18700.153312999984</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>262</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>14803.396081000006</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>262</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>16983.844487000006</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>262</v>
       </c>
@@ -4563,7 +4565,7 @@
         <v>52466.281798000004</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>262</v>
       </c>
@@ -4586,7 +4588,7 @@
         <v>68282.789418699991</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>262</v>
       </c>
@@ -4594,7 +4596,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>262</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>262</v>
       </c>
@@ -4625,7 +4627,7 @@
         <v>17165.98502</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>262</v>
       </c>
@@ -4648,7 +4650,7 @@
         <v>37733.163335299985</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>262</v>
       </c>
@@ -4656,7 +4658,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>262</v>
       </c>
@@ -4669,7 +4671,7 @@
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>262</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v>63143.517413999907</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>262</v>
       </c>
@@ -4715,7 +4717,7 @@
         <v>61608.056062299991</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>262</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>44717.73671200002</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>262</v>
       </c>
@@ -4761,7 +4763,7 @@
         <v>76477.072908000046</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>262</v>
       </c>
@@ -4784,7 +4786,7 @@
         <v>37629.551669</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>262</v>
       </c>
@@ -4807,7 +4809,7 @@
         <v>28793.63652630003</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
         <v>262</v>
       </c>
@@ -4830,7 +4832,7 @@
         <v>26331.084063699971</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
         <v>262</v>
       </c>
@@ -4853,7 +4855,7 @@
         <v>40366.639767999972</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
         <v>262</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>32808.833446999968</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
         <v>262</v>
       </c>
@@ -4899,7 +4901,7 @@
         <v>47757.485666</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
         <v>262</v>
       </c>
@@ -4922,7 +4924,7 @@
         <v>27015.48869100001</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
         <v>262</v>
       </c>
@@ -4945,7 +4947,7 @@
         <v>31854.632514700017</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
         <v>262</v>
       </c>
@@ -4968,7 +4970,7 @@
         <v>68132.192042299939</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A174" t="s">
         <v>262</v>
       </c>
@@ -4991,7 +4993,7 @@
         <v>38708.725029500005</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
         <v>262</v>
       </c>
@@ -5014,7 +5016,7 @@
         <v>48908.07160500007</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
         <v>262</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>59453.078786999904</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>262</v>
       </c>
@@ -5060,7 +5062,7 @@
         <v>54923.321220999918</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>262</v>
       </c>
@@ -5083,7 +5085,7 @@
         <v>22587.152666300008</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>262</v>
       </c>
@@ -5106,7 +5108,7 @@
         <v>36553.220813999971</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
         <v>262</v>
       </c>
@@ -5129,7 +5131,7 @@
         <v>36339.247396000021</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>262</v>
       </c>
@@ -5152,7 +5154,7 @@
         <v>68214.208321999802</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
         <v>262</v>
       </c>
@@ -5175,7 +5177,7 @@
         <v>23583.758151000031</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
         <v>262</v>
       </c>
@@ -5198,7 +5200,7 @@
         <v>31964.300209000045</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
         <v>262</v>
       </c>
@@ -5221,7 +5223,7 @@
         <v>73044.647955999913</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
         <v>262</v>
       </c>
@@ -5244,7 +5246,7 @@
         <v>51693.983547000098</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
         <v>262</v>
       </c>
@@ -5267,7 +5269,7 @@
         <v>42698.36343499997</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A187" t="s">
         <v>262</v>
       </c>
@@ -5290,7 +5292,7 @@
         <v>63447.958487000076</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A188" t="s">
         <v>262</v>
       </c>
@@ -5313,7 +5315,7 @@
         <v>28273.919575999975</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A189" t="s">
         <v>262</v>
       </c>
@@ -5336,7 +5338,7 @@
         <v>61477.377808999991</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A190" t="s">
         <v>262</v>
       </c>
@@ -5359,7 +5361,7 @@
         <v>68135.713886999962</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A191" t="s">
         <v>262</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>70430.819512999893</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>262</v>
       </c>
@@ -5405,7 +5407,7 @@
         <v>45292.045241000036</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A193" t="s">
         <v>262</v>
       </c>
@@ -5428,7 +5430,7 @@
         <v>22727.8274423</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
         <v>262</v>
       </c>
@@ -5451,7 +5453,7 @@
         <v>20823.100282299998</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A195" t="s">
         <v>262</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>71567.174660000019</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A196" t="s">
         <v>262</v>
       </c>
@@ -5497,7 +5499,7 @@
         <v>34306.547029000008</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
         <v>262</v>
       </c>
@@ -5520,7 +5522,7 @@
         <v>43854.571700999972</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>262</v>
       </c>
@@ -5543,7 +5545,7 @@
         <v>32999.012674999991</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A199" t="s">
         <v>262</v>
       </c>
@@ -5566,7 +5568,7 @@
         <v>66856.267311000091</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A200" t="s">
         <v>262</v>
       </c>
@@ -5589,7 +5591,7 @@
         <v>70959.576349999988</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A201" t="s">
         <v>262</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>19321.060838300007</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A202" t="s">
         <v>262</v>
       </c>
@@ -5635,7 +5637,7 @@
         <v>63516.994559000064</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
         <v>262</v>
       </c>
@@ -5658,7 +5660,7 @@
         <v>26133.694736000001</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
         <v>262</v>
       </c>
@@ -5682,7 +5684,7 @@
         <v>26670.627858</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
         <v>262</v>
       </c>
@@ -5705,7 +5707,7 @@
         <v>69290.364170999965</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A206" t="s">
         <v>262</v>
       </c>
@@ -5728,7 +5730,7 @@
         <v>16947.531448999995</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A207" t="s">
         <v>262</v>
       </c>
@@ -5751,7 +5753,7 @@
         <v>58020.507783999929</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A208" t="s">
         <v>262</v>
       </c>
@@ -5774,7 +5776,7 @@
         <v>30219.618571000039</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A209" t="s">
         <v>262</v>
       </c>
@@ -5797,7 +5799,7 @@
         <v>42630.40016499997</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A210" t="s">
         <v>262</v>
       </c>
@@ -5820,7 +5822,7 @@
         <v>41673.214780999981</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A211" t="s">
         <v>262</v>
       </c>
@@ -5843,7 +5845,7 @@
         <v>51253.019620299987</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A212" t="s">
         <v>262</v>
       </c>
@@ -5866,7 +5868,7 @@
         <v>29282.284593500019</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
         <v>262</v>
       </c>
@@ -5889,7 +5891,7 @@
         <v>35904.378373000014</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A214" t="s">
         <v>262</v>
       </c>
@@ -5912,7 +5914,7 @@
         <v>54046.477851000047</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A215" t="s">
         <v>262</v>
       </c>
@@ -5935,7 +5937,7 @@
         <v>42773.671616000065</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A216" t="s">
         <v>262</v>
       </c>
@@ -5958,7 +5960,7 @@
         <v>51950.046098599996</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A217" t="s">
         <v>262</v>
       </c>
@@ -5981,7 +5983,7 @@
         <v>20825.033415999995</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A218" t="s">
         <v>262</v>
       </c>
@@ -6004,7 +6006,7 @@
         <v>44602.461408999872</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A219" t="s">
         <v>262</v>
       </c>
@@ -6027,7 +6029,7 @@
         <v>41020.388355699914</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A220" t="s">
         <v>262</v>
       </c>
@@ -6050,7 +6052,7 @@
         <v>22072.295252000022</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A221" t="s">
         <v>262</v>
       </c>
@@ -6073,7 +6075,7 @@
         <v>27554.725491999998</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A222" t="s">
         <v>262</v>
       </c>
@@ -6096,7 +6098,7 @@
         <v>20010.450242000003</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A223" t="s">
         <v>262</v>
       </c>
@@ -6119,7 +6121,7 @@
         <v>37870.7215603</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>262</v>
       </c>
@@ -6142,7 +6144,7 @@
         <v>68415.723105999932</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A225" t="s">
         <v>262</v>
       </c>
@@ -6165,7 +6167,7 @@
         <v>46007.571995000006</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A226" t="s">
         <v>262</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>28579.348239000021</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A227" t="s">
         <v>262</v>
       </c>
@@ -6211,7 +6213,7 @@
         <v>36552.907583999964</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A228" t="s">
         <v>262</v>
       </c>
@@ -6234,7 +6236,7 @@
         <v>62160.991679999912</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A229" t="s">
         <v>262</v>
       </c>
@@ -6257,7 +6259,7 @@
         <v>13522.912074000002</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A230" t="s">
         <v>262</v>
       </c>
@@ -6280,7 +6282,7 @@
         <v>62705.011036500022</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A231" t="s">
         <v>262</v>
       </c>
@@ -6303,7 +6305,7 @@
         <v>68638.103165000211</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A232" t="s">
         <v>262</v>
       </c>
@@ -6326,7 +6328,7 @@
         <v>76346.118259000083</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A233" t="s">
         <v>262</v>
       </c>
@@ -6349,7 +6351,7 @@
         <v>46465.82569299997</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A234" t="s">
         <v>262</v>
       </c>
@@ -6372,7 +6374,7 @@
         <v>25846.164582000019</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A235" t="s">
         <v>262</v>
       </c>
@@ -6395,7 +6397,7 @@
         <v>41811.401943999939</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A236" t="s">
         <v>262</v>
       </c>
@@ -6418,7 +6420,7 @@
         <v>26402.751604499997</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A237" t="s">
         <v>262</v>
       </c>
@@ -6441,7 +6443,7 @@
         <v>27048.232333999993</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A238" t="s">
         <v>262</v>
       </c>
@@ -6464,7 +6466,7 @@
         <v>23536.021755999984</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A239" t="s">
         <v>262</v>
       </c>
@@ -6487,7 +6489,7 @@
         <v>60697.166624600046</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>262</v>
       </c>
@@ -6510,7 +6512,7 @@
         <v>59737.899550800066</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A241" t="s">
         <v>262</v>
       </c>
@@ -6533,7 +6535,7 @@
         <v>54866.181939999973</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A242" t="s">
         <v>262</v>
       </c>
@@ -6556,7 +6558,7 @@
         <v>25792.034221000027</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>262</v>
       </c>
@@ -6579,7 +6581,7 @@
         <v>38207.878221999992</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A244" t="s">
         <v>262</v>
       </c>
@@ -6602,7 +6604,7 @@
         <v>47061.678981000121</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A245" t="s">
         <v>262</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>56589.282591299983</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A246" t="s">
         <v>262</v>
       </c>
@@ -6648,7 +6650,7 @@
         <v>63787.708169300058</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A247" t="s">
         <v>262</v>
       </c>
@@ -6671,7 +6673,7 @@
         <v>71269.211713000026</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A248" t="s">
         <v>262</v>
       </c>
@@ -6694,7 +6696,7 @@
         <v>49958.490934000016</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A249" t="s">
         <v>262</v>
       </c>
@@ -6717,7 +6719,7 @@
         <v>33278.835616000026</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A250" t="s">
         <v>262</v>
       </c>
@@ -6740,7 +6742,7 @@
         <v>58575.632935999995</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A251" t="s">
         <v>262</v>
       </c>
@@ -6763,7 +6765,7 @@
         <v>72142.282425300073</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A252" t="s">
         <v>262</v>
       </c>
@@ -6786,7 +6788,7 @@
         <v>73354.28465229999</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A253" t="s">
         <v>262</v>
       </c>
@@ -6809,7 +6811,7 @@
         <v>57659.651555000011</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A254" t="s">
         <v>262</v>
       </c>
@@ -6832,7 +6834,7 @@
         <v>32293.159831000012</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A255" t="s">
         <v>262</v>
       </c>
@@ -6855,7 +6857,7 @@
         <v>61154.89756400005</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A256" t="s">
         <v>262</v>
       </c>

</xml_diff>